<commit_message>
Allocated Tasks to team members in sheet
</commit_message>
<xml_diff>
--- a/Planning and Design/Burndown Chart, Back Log, Product Log.xlsx
+++ b/Planning and Design/Burndown Chart, Back Log, Product Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjpra\Documents\GCU\CST 247\Milestone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjpra\Documents\GCU\CST 247\Milestone\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99A26E8-8CA6-4797-9459-89BB676C53E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D80CDD4-837D-4634-B136-9696703FD829}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Assigned To</t>
   </si>
   <si>
-    <t>Team Member</t>
-  </si>
-  <si>
     <t>User Story</t>
   </si>
   <si>
@@ -153,78 +150,84 @@
     <t>Create registration form for new players</t>
   </si>
   <si>
-    <t xml:space="preserve">Project Title: Minesweeper CLC Milestone
+    <t>Create Database to store players</t>
+  </si>
+  <si>
+    <t>As a player I would like the site to be secure so that my login information is safe</t>
+  </si>
+  <si>
+    <t>As a user I would like to have an ability to login to the site</t>
+  </si>
+  <si>
+    <t>Create a Login Page wher users can create username and passwords</t>
+  </si>
+  <si>
+    <t>Store users login information within a database</t>
+  </si>
+  <si>
+    <t>Add security to the site to protect user information</t>
+  </si>
+  <si>
+    <t>As a player I want to save my game data and stats</t>
+  </si>
+  <si>
+    <t>Connect players game stats and data to the database</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to see my stats displayed on the screen</t>
+  </si>
+  <si>
+    <t>Display game stats and results on screen</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to see my old stats</t>
+  </si>
+  <si>
+    <t>Retrieve stats stored in database</t>
+  </si>
+  <si>
+    <t>Desired Features</t>
+  </si>
+  <si>
+    <t>Register New Users</t>
+  </si>
+  <si>
+    <t>Login to Game Site</t>
+  </si>
+  <si>
+    <t>Make Site Secure</t>
+  </si>
+  <si>
+    <t>Save Game Stats in database</t>
+  </si>
+  <si>
+    <t>Display Game Stats</t>
+  </si>
+  <si>
+    <t>Retrieve Stats from database</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t>4 hrs</t>
+  </si>
+  <si>
+    <t>1 hrs</t>
+  </si>
+  <si>
+    <t>Project Title: Minesweeper CLC Milestone
 Release #:
-Sprint #: </t>
-  </si>
-  <si>
-    <t>Create Database to store players</t>
-  </si>
-  <si>
-    <t>As a player I would like the site to be secure so that my login information is safe</t>
-  </si>
-  <si>
-    <t>As a user I would like to have an ability to login to the site</t>
-  </si>
-  <si>
-    <t>Create a Login Page wher users can create username and passwords</t>
-  </si>
-  <si>
-    <t>Store users login information within a database</t>
-  </si>
-  <si>
-    <t>Add security to the site to protect user information</t>
-  </si>
-  <si>
-    <t>As a player I want to save my game data and stats</t>
-  </si>
-  <si>
-    <t>Connect players game stats and data to the database</t>
-  </si>
-  <si>
-    <t>As a player I want to be able to see my stats displayed on the screen</t>
-  </si>
-  <si>
-    <t>Display game stats and results on screen</t>
-  </si>
-  <si>
-    <t>As a player I want to be able to see my old stats</t>
-  </si>
-  <si>
-    <t>Retrieve stats stored in database</t>
-  </si>
-  <si>
-    <t>Desired Features</t>
-  </si>
-  <si>
-    <t>Register New Users</t>
-  </si>
-  <si>
-    <t>Login to Game Site</t>
-  </si>
-  <si>
-    <t>Make Site Secure</t>
-  </si>
-  <si>
-    <t>Save Game Stats in database</t>
-  </si>
-  <si>
-    <t>Display Game Stats</t>
-  </si>
-  <si>
-    <t>Retrieve Stats from database</t>
-  </si>
-  <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
-    <t>4 hrs</t>
-  </si>
-  <si>
-    <t>1 hrs</t>
+Sprint #: 1</t>
+  </si>
+  <si>
+    <t>Mark Pratt</t>
+  </si>
+  <si>
+    <t>Patrick Garcia</t>
   </si>
 </sst>
 </file>
@@ -483,14 +486,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,6 +513,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,70 +950,6 @@
           </cell>
           <cell r="O5" t="str">
             <v>Day 1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>27</v>
-          </cell>
-          <cell r="G19">
-            <v>24</v>
-          </cell>
-          <cell r="H19">
-            <v>21</v>
-          </cell>
-          <cell r="I19">
-            <v>18</v>
-          </cell>
-          <cell r="J19">
-            <v>15</v>
-          </cell>
-          <cell r="K19">
-            <v>12</v>
-          </cell>
-          <cell r="L19">
-            <v>9</v>
-          </cell>
-          <cell r="M19">
-            <v>6</v>
-          </cell>
-          <cell r="N19">
-            <v>3</v>
-          </cell>
-          <cell r="O19">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>29</v>
-          </cell>
-          <cell r="G20">
-            <v>27</v>
-          </cell>
-          <cell r="H20">
-            <v>21</v>
-          </cell>
-          <cell r="I20">
-            <v>21</v>
-          </cell>
-          <cell r="J20">
-            <v>17</v>
-          </cell>
-          <cell r="K20">
-            <v>17</v>
-          </cell>
-          <cell r="L20">
-            <v>11</v>
-          </cell>
-          <cell r="M20">
-            <v>6</v>
-          </cell>
-          <cell r="N20">
-            <v>6</v>
-          </cell>
-          <cell r="O20">
-            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -1286,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1299,15 +1238,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="A1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1335,7 +1274,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1385,13 +1324,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F4" s="4">
         <v>2</v>
@@ -1434,10 +1373,10 @@
       <c r="B5" s="7"/>
       <c r="C5" s="10"/>
       <c r="D5" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -1481,13 +1420,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F6" s="4">
         <v>4</v>
@@ -1530,10 +1469,10 @@
       <c r="B7" s="7"/>
       <c r="C7" s="10"/>
       <c r="D7" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -1577,13 +1516,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
@@ -1627,13 +1566,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -1677,13 +1616,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1727,13 +1666,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1773,12 +1712,12 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="4">
         <f>SUM(F4:F11)</f>
         <v>18</v>
@@ -1828,12 +1767,12 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="4">
         <f>SUM(F4:F11)</f>
         <v>18</v>
@@ -2352,75 +2291,75 @@
   <sheetData>
     <row r="3" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="4:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D11" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="D5" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="D9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.35">
-      <c r="D10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="4:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="D11" s="18" t="s">
+    <row r="12" spans="4:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="4:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>59</v>
+      <c r="E12" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2446,38 +2385,38 @@
   <sheetData>
     <row r="3" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D5" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D6" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D5" s="21" t="s">
+    <row r="7" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D7" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D6" s="22" t="s">
+    <row r="8" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D8" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D7" s="22" t="s">
+    <row r="9" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D8" s="22" t="s">
+    <row r="10" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="20" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D9" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D10" s="23" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2499,74 +2438,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated Burndown Chart for Week 3
</commit_message>
<xml_diff>
--- a/Planning and Design/Burndown Chart, Back Log, Product Log.xlsx
+++ b/Planning and Design/Burndown Chart, Back Log, Product Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjpra\Documents\GCU\CST 247\Milestone\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D80CDD4-837D-4634-B136-9696703FD829}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C259111-C878-4A9F-B5D0-D88DEBCC2423}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
   <si>
     <t>Task</t>
   </si>
@@ -217,17 +217,26 @@
   </si>
   <si>
     <t>1 hrs</t>
+  </si>
+  <si>
+    <t>Mark Pratt</t>
+  </si>
+  <si>
+    <t>Patrick Garcia</t>
   </si>
   <si>
     <t>Project Title: Minesweeper CLC Milestone
 Release #:
-Sprint #: 1</t>
-  </si>
-  <si>
-    <t>Mark Pratt</t>
-  </si>
-  <si>
-    <t>Patrick Garcia</t>
+Sprint #: 2</t>
+  </si>
+  <si>
+    <t>As a player, I need to log in to the site in order to play the game</t>
+  </si>
+  <si>
+    <t>After log in page, bring up game board</t>
+  </si>
+  <si>
+    <t>Connect site to game logic</t>
   </si>
 </sst>
 </file>
@@ -643,42 +652,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$12:$P$12</c:f>
+              <c:f>'Burn Down Chart'!$F$14:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.2</c:v>
+                  <c:v>24.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.399999999999999</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.599999999999998</c:v>
+                  <c:v>18.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.799999999999997</c:v>
+                  <c:v>16.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.9999999999999964</c:v>
+                  <c:v>13.500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.1999999999999966</c:v>
+                  <c:v>10.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3999999999999968</c:v>
+                  <c:v>8.100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.599999999999997</c:v>
+                  <c:v>5.4000000000000048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7999999999999969</c:v>
+                  <c:v>2.7000000000000046</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.1086244689504383E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,42 +766,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$13:$P$13</c:f>
+              <c:f>'Burn Down Chart'!$F$15:$P$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,13 +882,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1223,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,7 +1248,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -1330,41 +1339,23 @@
         <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="4">
         <v>2</v>
       </c>
       <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4">
-        <v>0</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
@@ -1376,41 +1367,23 @@
         <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
@@ -1426,41 +1399,23 @@
         <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0</v>
-      </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
@@ -1472,41 +1427,23 @@
         <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0</v>
-      </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
@@ -1522,41 +1459,21 @@
         <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <v>0</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
-        <v>0</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
@@ -1572,41 +1489,21 @@
         <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <v>0</v>
-      </c>
-      <c r="O9" s="4">
-        <v>0</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
@@ -1622,41 +1519,21 @@
         <v>45</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="4">
-        <v>0</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1672,191 +1549,191 @@
         <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0</v>
-      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="B12" s="7">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="4">
-        <f>SUM(F4:F11)</f>
-        <v>18</v>
-      </c>
-      <c r="G12" s="4">
-        <f>F12-$F$12/10</f>
-        <v>16.2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="4">
-        <f t="shared" ref="H12:P12" si="0">G12-$F$12/10</f>
-        <v>14.399999999999999</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="0"/>
-        <v>12.599999999999998</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="0"/>
-        <v>10.799999999999997</v>
-      </c>
-      <c r="K12" s="4">
-        <f t="shared" si="0"/>
-        <v>8.9999999999999964</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" si="0"/>
-        <v>7.1999999999999966</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="0"/>
-        <v>5.3999999999999968</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" si="0"/>
-        <v>3.599999999999997</v>
-      </c>
-      <c r="O12" s="4">
-        <f t="shared" si="0"/>
-        <v>1.7999999999999969</v>
-      </c>
-      <c r="P12" s="4">
-        <f t="shared" si="0"/>
-        <v>-3.1086244689504383E-15</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="4">
-        <f>SUM(F4:F11)</f>
-        <v>18</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" ref="G13:P13" si="1">F13 - SUM(G4:G11)</f>
-        <v>18</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="N13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="O13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="P13" s="4">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="B14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="4">
+        <f>SUM(F4:F13)</f>
+        <v>27</v>
+      </c>
+      <c r="G14" s="4">
+        <f>F14-$F$14/10</f>
+        <v>24.3</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" ref="H14:O14" si="0">G14-$F$14/10</f>
+        <v>21.6</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>18.900000000000002</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>16.200000000000003</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="0"/>
+        <v>13.500000000000004</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="0"/>
+        <v>10.800000000000004</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="0"/>
+        <v>8.100000000000005</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="0"/>
+        <v>5.4000000000000048</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000046</v>
+      </c>
+      <c r="P14" s="4">
+        <f>IF((O14-$F$14/10) &gt;= 1, (O14-$F$14/10), 0)</f>
+        <v>0</v>
+      </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="B15" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="4">
+        <f>SUM(F4:F13)</f>
+        <v>27</v>
+      </c>
+      <c r="G15" s="4">
+        <f>F15 - SUM(G4:G13)</f>
+        <v>19</v>
+      </c>
+      <c r="H15" s="4">
+        <f>G15 - SUM(H4:H13)</f>
+        <v>7</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" ref="I15:P15" si="1">H15 - SUM(I4:I13)</f>
+        <v>7</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
@@ -2260,10 +2137,50 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>